<commit_message>
Jinja2 templates working for EC2
</commit_message>
<xml_diff>
--- a/FG-47856.xlsx
+++ b/FG-47856.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
   <si>
     <t>ServerType</t>
   </si>
@@ -91,6 +91,9 @@
     <t>xx-sd2a:d</t>
   </si>
   <si>
+    <t>us-east-1</t>
+  </si>
+  <si>
     <t>Postgres</t>
   </si>
   <si>
@@ -133,6 +136,9 @@
     <t>xx-sd4b</t>
   </si>
   <si>
+    <t>us-west-1</t>
+  </si>
+  <si>
     <t>ami-1111111</t>
   </si>
   <si>
@@ -161,6 +167,9 @@
   </si>
   <si>
     <t>xx-sd6b</t>
+  </si>
+  <si>
+    <t>us-central-2</t>
   </si>
   <si>
     <t>ami-2222222</t>
@@ -589,43 +598,45 @@
       <c r="C2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G2" s="4">
         <v>11.1</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I2" s="4">
         <v>1200.0</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="T2" s="8">
         <v>700.0</v>
@@ -634,67 +645,69 @@
         <v>2100.0</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="W2" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="E3" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G3" s="4">
         <v>2016.0</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I3" s="4">
         <v>150.0</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P3" s="4">
         <v>200.0</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="T3" s="8">
         <v>700.0</v>
@@ -703,67 +716,69 @@
         <v>1700.0</v>
       </c>
       <c r="V3" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="4"/>
+        <v>51</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="E4" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G4" s="4">
         <v>2016.0</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I4" s="4">
         <v>150.0</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="P4" s="4">
         <v>150.0</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="T4" s="8">
         <v>700.0</v>
@@ -772,10 +787,10 @@
         <v>1700.0</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>